<commit_message>
Modelos finales y baselines
</commit_message>
<xml_diff>
--- a/models/Baselines/all_results.xlsx
+++ b/models/Baselines/all_results.xlsx
@@ -14,12 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="33">
   <si>
     <t>Position</t>
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>NDCG@-1</t>
+  </si>
+  <si>
+    <t>NDCG@1</t>
+  </si>
+  <si>
+    <t>NDCG@10</t>
   </si>
   <si>
     <t>F1@1</t>
@@ -461,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,2957 +516,3614 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2">
+        <v>0.621239185333252</v>
+      </c>
+      <c r="D2">
         <v>0.4347457587718963</v>
       </c>
-      <c r="D2">
-        <v>0.2104519804318746</v>
-      </c>
       <c r="E2">
-        <v>0.1298921359472037</v>
+        <v>0.5644705295562744</v>
       </c>
       <c r="F2">
         <v>0.4347457587718963</v>
       </c>
       <c r="G2">
-        <v>0.1262711882591247</v>
+        <v>0.2104519804318746</v>
       </c>
       <c r="H2">
-        <v>0.0714406743645668</v>
+        <v>0.1298921359472037</v>
       </c>
       <c r="I2">
         <v>0.4347457587718963</v>
       </c>
       <c r="J2">
+        <v>0.1262711882591247</v>
+      </c>
+      <c r="K2">
+        <v>0.0714406743645668</v>
+      </c>
+      <c r="L2">
+        <v>0.4347457587718963</v>
+      </c>
+      <c r="M2">
         <v>0.6313559412956238</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>0.7144067883491516</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3">
+        <v>0.6429080367088318</v>
+      </c>
+      <c r="D3">
         <v>0.4338982999324798</v>
       </c>
-      <c r="D3">
-        <v>0.2268361565139558</v>
-      </c>
       <c r="E3">
-        <v>0.1410631699995561</v>
+        <v>0.5952140688896179</v>
       </c>
       <c r="F3">
         <v>0.4338982999324798</v>
       </c>
       <c r="G3">
-        <v>0.1361016929149627</v>
+        <v>0.2268361565139558</v>
       </c>
       <c r="H3">
-        <v>0.0775847434997558</v>
+        <v>0.1410631699995561</v>
       </c>
       <c r="I3">
         <v>0.4338982999324798</v>
       </c>
       <c r="J3">
+        <v>0.1361016929149627</v>
+      </c>
+      <c r="K3">
+        <v>0.0775847434997558</v>
+      </c>
+      <c r="L3">
+        <v>0.4338982999324798</v>
+      </c>
+      <c r="M3">
         <v>0.6805084943771362</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>0.7758474349975586</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>0.380084753036499</v>
+        <v>0.5974993705749512</v>
       </c>
       <c r="D4">
-        <v>0.2074858786331282</v>
+        <v>0.3796610236167907</v>
       </c>
       <c r="E4">
-        <v>0.1312018524516712</v>
+        <v>0.5396417379379272</v>
       </c>
       <c r="F4">
         <v>0.380084753036499</v>
       </c>
       <c r="G4">
-        <v>0.1244915276765823</v>
+        <v>0.2074858786331282</v>
       </c>
       <c r="H4">
-        <v>0.07216101884841911</v>
+        <v>0.1312018524516712</v>
       </c>
       <c r="I4">
         <v>0.380084753036499</v>
       </c>
       <c r="J4">
+        <v>0.1244915276765823</v>
+      </c>
+      <c r="K4">
+        <v>0.07216101884841911</v>
+      </c>
+      <c r="L4">
+        <v>0.380084753036499</v>
+      </c>
+      <c r="M4">
         <v>0.6224576234817505</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>0.7216101884841919</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5">
+        <v>0.3011026262689675</v>
+      </c>
+      <c r="D5">
+        <v>0.0757674722403657</v>
+      </c>
+      <c r="E5">
+        <v>0.1553376253333435</v>
+      </c>
+      <c r="F5">
         <v>0.06855359605196309</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>0.0698198183991781</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>0.0583497207950461</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>0.0757674722403657</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>0.0455911169170479</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>0.0339647289353366</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>0.06577944698454161</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>0.1772780760860448</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>0.260701090403899</v>
       </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="P5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6">
+        <v>0.3061950541106025</v>
+      </c>
+      <c r="D6">
+        <v>0.07054212932723709</v>
+      </c>
+      <c r="E6">
+        <v>0.161341616752191</v>
+      </c>
+      <c r="F6">
         <v>0.0639161042165614</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>0.0708349147767826</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>0.0601267097951213</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>0.07054212932723709</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>0.0457217504898761</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>0.0349444807315483</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>0.0614794252122795</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>0.1856603970091886</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>0.2714817768050949</v>
       </c>
-      <c r="L6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7">
+        <v>0.306276243378811</v>
+      </c>
+      <c r="D7">
+        <v>0.07054212932723709</v>
+      </c>
+      <c r="E7">
+        <v>0.1617108665390191</v>
+      </c>
+      <c r="F7">
         <v>0.0639161042165614</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>0.0708349147767826</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>0.0602786002002002</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>0.07054212932723709</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>0.0457217504898761</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>0.0350097975179624</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>0.0614794252122795</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>0.1856603970091886</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>0.2725073823049003</v>
       </c>
-      <c r="L7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="P7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8">
+        <v>0.5281693339347839</v>
+      </c>
+      <c r="D8">
         <v>0.3232499957084656</v>
       </c>
-      <c r="D8">
-        <v>0.176127676334646</v>
-      </c>
       <c r="E8">
-        <v>0.1110399720097376</v>
+        <v>0.4592688977718353</v>
       </c>
       <c r="F8">
         <v>0.3232499957084656</v>
       </c>
       <c r="G8">
-        <v>0.1056766062974929</v>
+        <v>0.176127676334646</v>
       </c>
       <c r="H8">
-        <v>0.0610719844698905</v>
+        <v>0.1110399720097376</v>
       </c>
       <c r="I8">
         <v>0.3232499957084656</v>
       </c>
       <c r="J8">
+        <v>0.1056766062974929</v>
+      </c>
+      <c r="K8">
+        <v>0.0610719844698905</v>
+      </c>
+      <c r="L8">
+        <v>0.3232499957084656</v>
+      </c>
+      <c r="M8">
         <v>0.5283830165863037</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>0.6107198596000671</v>
       </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9">
+        <v>0.4888517260551452</v>
+      </c>
+      <c r="D9">
         <v>0.286855399608612</v>
       </c>
-      <c r="D9">
-        <v>0.1597737529211574</v>
-      </c>
       <c r="E9">
-        <v>0.1014235549229235</v>
+        <v>0.4136734306812286</v>
       </c>
       <c r="F9">
         <v>0.286855399608612</v>
       </c>
       <c r="G9">
-        <v>0.09586425125598901</v>
+        <v>0.1597737529211574</v>
       </c>
       <c r="H9">
-        <v>0.0557829551398754</v>
+        <v>0.1014235549229235</v>
       </c>
       <c r="I9">
         <v>0.286855399608612</v>
       </c>
       <c r="J9">
+        <v>0.09586425125598901</v>
+      </c>
+      <c r="K9">
+        <v>0.0557829551398754</v>
+      </c>
+      <c r="L9">
+        <v>0.286855399608612</v>
+      </c>
+      <c r="M9">
         <v>0.4793212711811065</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>0.5578295588493347</v>
       </c>
-      <c r="L9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0.2844448685646057</v>
+        <v>0.4877307713031769</v>
       </c>
       <c r="D10">
-        <v>0.1594113806883494</v>
+        <v>0.2842558026313782</v>
       </c>
       <c r="E10">
-        <v>0.1016985562222062</v>
+        <v>0.4130165576934814</v>
       </c>
       <c r="F10">
         <v>0.2844448685646057</v>
       </c>
       <c r="G10">
-        <v>0.0956468284130096</v>
+        <v>0.1594113806883494</v>
       </c>
       <c r="H10">
-        <v>0.0559342056512832</v>
+        <v>0.1016985562222062</v>
       </c>
       <c r="I10">
         <v>0.2844448685646057</v>
       </c>
       <c r="J10">
+        <v>0.0956468284130096</v>
+      </c>
+      <c r="K10">
+        <v>0.0559342056512832</v>
+      </c>
+      <c r="L10">
+        <v>0.2844448685646057</v>
+      </c>
+      <c r="M10">
         <v>0.4782341420650482</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>0.559342086315155</v>
       </c>
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11">
+        <v>0.18226741416395</v>
+      </c>
+      <c r="D11">
+        <v>0.0259686385132332</v>
+      </c>
+      <c r="E11">
+        <v>0.0480916198860152</v>
+      </c>
+      <c r="F11">
         <v>0.0210106775144524</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>0.0218782181185206</v>
       </c>
-      <c r="E11">
+      <c r="H11">
         <v>0.0189384201826741</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>0.0259686385132332</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>0.0149838214552392</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>0.0113996515390356</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>0.0194280469929113</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>0.0523254500640624</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>0.07759919447105119</v>
       </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12">
+        <v>0.1667009797255122</v>
+      </c>
+      <c r="D12">
+        <v>0.0119472330540114</v>
+      </c>
+      <c r="E12">
+        <v>0.0302430221869163</v>
+      </c>
+      <c r="F12">
         <v>0.0093980877387498</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>0.0140204263814922</v>
       </c>
-      <c r="E12">
+      <c r="H12">
         <v>0.0134851677674742</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <v>0.0119472330540114</v>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>0.009624159960175901</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>0.0081639425869077</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>0.008607541009897499</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>0.0333994725937572</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>0.054751128669103</v>
       </c>
-      <c r="L12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="O12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C13">
+        <v>0.1666986580391633</v>
+      </c>
+      <c r="D13">
+        <v>0.0119472330540114</v>
+      </c>
+      <c r="E13">
+        <v>0.0302402646691383</v>
+      </c>
+      <c r="F13">
         <v>0.0093980877387498</v>
       </c>
-      <c r="D13">
+      <c r="G13">
         <v>0.0140204263814922</v>
       </c>
-      <c r="E13">
+      <c r="H13">
         <v>0.0134851677674742</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <v>0.0119472330540114</v>
       </c>
-      <c r="G13">
+      <c r="J13">
         <v>0.009624159960175901</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>0.0081639425869077</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>0.008607541009897499</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>0.0333994725937572</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>0.054751128669103</v>
       </c>
-      <c r="L13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C14">
+        <v>0.572415292263031</v>
+      </c>
+      <c r="D14">
         <v>0.3791394829750061</v>
       </c>
-      <c r="D14">
-        <v>0.1944786413676207</v>
-      </c>
       <c r="E14">
-        <v>0.1198952449254752</v>
+        <v>0.5126505494117737</v>
       </c>
       <c r="F14">
         <v>0.3791394829750061</v>
       </c>
       <c r="G14">
-        <v>0.1166871860623359</v>
+        <v>0.1944786413676207</v>
       </c>
       <c r="H14">
-        <v>0.06594238430261611</v>
+        <v>0.1198952449254752</v>
       </c>
       <c r="I14">
         <v>0.3791394829750061</v>
       </c>
       <c r="J14">
+        <v>0.1166871860623359</v>
+      </c>
+      <c r="K14">
+        <v>0.06594238430261611</v>
+      </c>
+      <c r="L14">
+        <v>0.3791394829750061</v>
+      </c>
+      <c r="M14">
         <v>0.5834358930587769</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>0.6594238877296448</v>
       </c>
-      <c r="L14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="O14" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>0.3532254099845886</v>
+        <v>0.5445130467414856</v>
       </c>
       <c r="D15">
-        <v>0.1826603454020288</v>
+        <v>0.3528560996055603</v>
       </c>
       <c r="E15">
-        <v>0.1129844575381475</v>
+        <v>0.4808982312679291</v>
       </c>
       <c r="F15">
         <v>0.3532254099845886</v>
       </c>
       <c r="G15">
-        <v>0.1095962077379226</v>
+        <v>0.1826603454020288</v>
       </c>
       <c r="H15">
-        <v>0.0621414519846439</v>
+        <v>0.1129844575381475</v>
       </c>
       <c r="I15">
         <v>0.3532254099845886</v>
       </c>
       <c r="J15">
+        <v>0.1095962077379226</v>
+      </c>
+      <c r="K15">
+        <v>0.0621414519846439</v>
+      </c>
+      <c r="L15">
+        <v>0.3532254099845886</v>
+      </c>
+      <c r="M15">
         <v>0.5479810237884521</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>0.6214144825935364</v>
       </c>
-      <c r="L15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="O15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>0.3301120400428772</v>
+        <v>0.5249127745628357</v>
       </c>
       <c r="D16">
-        <v>0.1746891558998161</v>
+        <v>0.3300812542438507</v>
       </c>
       <c r="E16">
-        <v>0.1088435745928898</v>
+        <v>0.4573675394058227</v>
       </c>
       <c r="F16">
         <v>0.3301120400428772</v>
       </c>
       <c r="G16">
-        <v>0.1048134937882423</v>
+        <v>0.1746891558998161</v>
       </c>
       <c r="H16">
-        <v>0.0598639659583568</v>
+        <v>0.1088435745928898</v>
       </c>
       <c r="I16">
         <v>0.3301120400428772</v>
       </c>
       <c r="J16">
+        <v>0.1048134937882423</v>
+      </c>
+      <c r="K16">
+        <v>0.0598639659583568</v>
+      </c>
+      <c r="L16">
+        <v>0.3301120400428772</v>
+      </c>
+      <c r="M16">
         <v>0.5240674614906311</v>
       </c>
-      <c r="K16">
+      <c r="N16">
         <v>0.5986396670341492</v>
       </c>
-      <c r="L16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C17">
+        <v>0.1890690455557525</v>
+      </c>
+      <c r="D17">
+        <v>0.0282023089609675</v>
+      </c>
+      <c r="E17">
+        <v>0.0577890223456598</v>
+      </c>
+      <c r="F17">
         <v>0.0232382908049184</v>
       </c>
-      <c r="D17">
+      <c r="G17">
         <v>0.0273681715000765</v>
       </c>
-      <c r="E17">
+      <c r="H17">
         <v>0.023362388215715</v>
       </c>
-      <c r="F17">
+      <c r="I17">
         <v>0.0282023089609675</v>
       </c>
-      <c r="G17">
+      <c r="J17">
         <v>0.0187465640461786</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>0.01409565695437</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>0.021634963206214</v>
       </c>
-      <c r="J17">
+      <c r="M17">
         <v>0.065169563854597</v>
       </c>
-      <c r="K17">
+      <c r="N17">
         <v>0.0945103882975234</v>
       </c>
-      <c r="L17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="O17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C18">
+        <v>0.1755356807639797</v>
+      </c>
+      <c r="D18">
+        <v>0.0203958218801539</v>
+      </c>
+      <c r="E18">
+        <v>0.0415128552085981</v>
+      </c>
+      <c r="F18">
         <v>0.0164135551594021</v>
       </c>
-      <c r="D18">
+      <c r="G18">
         <v>0.0191942560050066</v>
       </c>
-      <c r="E18">
+      <c r="H18">
         <v>0.0171936062464999</v>
       </c>
-      <c r="F18">
+      <c r="I18">
         <v>0.0203958218801539</v>
       </c>
-      <c r="G18">
+      <c r="J18">
         <v>0.0131170973062119</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>0.0103573391973608</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>0.0151201984217956</v>
       </c>
-      <c r="J18">
+      <c r="M18">
         <v>0.0458760164508965</v>
       </c>
-      <c r="K18">
+      <c r="N18">
         <v>0.0705940538234434</v>
       </c>
-      <c r="L18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C19">
+        <v>0.1755265188191221</v>
+      </c>
+      <c r="D19">
+        <v>0.0203958218801539</v>
+      </c>
+      <c r="E19">
+        <v>0.0415128552085981</v>
+      </c>
+      <c r="F19">
         <v>0.0164135551594021</v>
       </c>
-      <c r="D19">
+      <c r="G19">
         <v>0.0191942560050066</v>
       </c>
-      <c r="E19">
+      <c r="H19">
         <v>0.0171936062464999</v>
       </c>
-      <c r="F19">
+      <c r="I19">
         <v>0.0203958218801539</v>
       </c>
-      <c r="G19">
+      <c r="J19">
         <v>0.0131170973062119</v>
       </c>
-      <c r="H19">
+      <c r="K19">
         <v>0.0103573391973608</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>0.0151201984217956</v>
       </c>
-      <c r="J19">
+      <c r="M19">
         <v>0.0458760164508965</v>
       </c>
-      <c r="K19">
+      <c r="N19">
         <v>0.0705940538234434</v>
       </c>
-      <c r="L19" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="O19" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C20">
-        <v>0.2854687869548797</v>
+        <v>0.4737207591533661</v>
       </c>
       <c r="D20">
-        <v>0.149907706098424</v>
+        <v>0.2854496836662292</v>
       </c>
       <c r="E20">
-        <v>0.0950023465412707</v>
+        <v>0.3960371315479278</v>
       </c>
       <c r="F20">
         <v>0.2854687869548797</v>
       </c>
       <c r="G20">
-        <v>0.0899446234107017</v>
+        <v>0.149907706098424</v>
       </c>
       <c r="H20">
-        <v>0.0522512905299663</v>
+        <v>0.0950023465412707</v>
       </c>
       <c r="I20">
         <v>0.2854687869548797</v>
       </c>
       <c r="J20">
+        <v>0.0899446234107017</v>
+      </c>
+      <c r="K20">
+        <v>0.0522512905299663</v>
+      </c>
+      <c r="L20">
+        <v>0.2854687869548797</v>
+      </c>
+      <c r="M20">
         <v>0.4497231245040893</v>
       </c>
-      <c r="K20">
+      <c r="N20">
         <v>0.5225129127502441</v>
       </c>
-      <c r="L20" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="O20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <v>0.2409394681453704</v>
+        <v>0.4258145093917846</v>
       </c>
       <c r="D21">
-        <v>0.1299726329743861</v>
+        <v>0.2409012764692306</v>
       </c>
       <c r="E21">
-        <v>0.0831808622710961</v>
+        <v>0.3411957621574402</v>
       </c>
       <c r="F21">
         <v>0.2409394681453704</v>
       </c>
       <c r="G21">
-        <v>0.07798358052968971</v>
+        <v>0.1299726329743861</v>
       </c>
       <c r="H21">
-        <v>0.0457494743168354</v>
+        <v>0.0831808622710961</v>
       </c>
       <c r="I21">
         <v>0.2409394681453704</v>
       </c>
       <c r="J21">
+        <v>0.07798358052968971</v>
+      </c>
+      <c r="K21">
+        <v>0.0457494743168354</v>
+      </c>
+      <c r="L21">
+        <v>0.2409394681453704</v>
+      </c>
+      <c r="M21">
         <v>0.3899178802967071</v>
       </c>
-      <c r="K21">
+      <c r="N21">
         <v>0.4574947357177734</v>
       </c>
-      <c r="L21" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="O21" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>0.2355356067419052</v>
+        <v>0.4205440580844879</v>
       </c>
       <c r="D22">
-        <v>0.1290879030194547</v>
+        <v>0.2352109998464584</v>
       </c>
       <c r="E22">
-        <v>0.0826288486315199</v>
+        <v>0.3372302055358886</v>
       </c>
       <c r="F22">
         <v>0.2355356067419052</v>
       </c>
       <c r="G22">
-        <v>0.0774527415633201</v>
+        <v>0.1290879030194547</v>
       </c>
       <c r="H22">
-        <v>0.045445866882801</v>
+        <v>0.0826288486315199</v>
       </c>
       <c r="I22">
         <v>0.2355356067419052</v>
       </c>
       <c r="J22">
+        <v>0.0774527415633201</v>
+      </c>
+      <c r="K22">
+        <v>0.045445866882801</v>
+      </c>
+      <c r="L22">
+        <v>0.2355356067419052</v>
+      </c>
+      <c r="M22">
         <v>0.3872637152671814</v>
       </c>
-      <c r="K22">
+      <c r="N22">
         <v>0.4544586539268493</v>
       </c>
-      <c r="L22" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="O22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C23">
+        <v>0.1560356507025002</v>
+      </c>
+      <c r="D23">
+        <v>0.0181102896289764</v>
+      </c>
+      <c r="E23">
+        <v>0.0350904415765707</v>
+      </c>
+      <c r="F23">
         <v>0.0141835127800377</v>
       </c>
-      <c r="D23">
+      <c r="G23">
         <v>0.0163397320749087</v>
       </c>
-      <c r="E23">
+      <c r="H23">
         <v>0.0142881192036416</v>
       </c>
-      <c r="F23">
+      <c r="I23">
         <v>0.0181102896289764</v>
       </c>
-      <c r="G23">
+      <c r="J23">
         <v>0.0112663636980258</v>
       </c>
-      <c r="H23">
+      <c r="K23">
         <v>0.008658346333853</v>
       </c>
-      <c r="I23">
+      <c r="L23">
         <v>0.0129234046311841</v>
       </c>
-      <c r="J23">
+      <c r="M23">
         <v>0.0386425503083608</v>
       </c>
-      <c r="K23">
+      <c r="N23">
         <v>0.0575789422216939</v>
       </c>
-      <c r="L23" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="O23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24">
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C24">
+        <v>0.1420312548045997</v>
+      </c>
+      <c r="D24">
+        <v>0.0141762192226819</v>
+      </c>
+      <c r="E24">
+        <v>0.0209680121113278</v>
+      </c>
+      <c r="F24">
         <v>0.0111791300412047</v>
       </c>
-      <c r="D24">
+      <c r="G24">
         <v>0.009419967431349799</v>
       </c>
-      <c r="E24">
+      <c r="H24">
         <v>0.0078504297800348</v>
       </c>
-      <c r="F24">
+      <c r="I24">
         <v>0.0141762192226819</v>
       </c>
-      <c r="G24">
+      <c r="J24">
         <v>0.0065047819304075</v>
       </c>
-      <c r="H24">
+      <c r="K24">
         <v>0.0047310588075695</v>
       </c>
-      <c r="I24">
+      <c r="L24">
         <v>0.0102124989052883</v>
       </c>
-      <c r="J24">
+      <c r="M24">
         <v>0.0222169829713439</v>
       </c>
-      <c r="K24">
+      <c r="N24">
         <v>0.0321644361979319</v>
       </c>
-      <c r="L24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="O24" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25">
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C25">
+        <v>0.1420487202789964</v>
+      </c>
+      <c r="D25">
+        <v>0.0141762192226819</v>
+      </c>
+      <c r="E25">
+        <v>0.0211671053053486</v>
+      </c>
+      <c r="F25">
         <v>0.0111791300412047</v>
       </c>
-      <c r="D25">
+      <c r="G25">
         <v>0.009419967431349799</v>
       </c>
-      <c r="E25">
+      <c r="H25">
         <v>0.007999242369568</v>
       </c>
-      <c r="F25">
+      <c r="I25">
         <v>0.0141762192226819</v>
       </c>
-      <c r="G25">
+      <c r="J25">
         <v>0.0065047819304075</v>
       </c>
-      <c r="H25">
+      <c r="K25">
         <v>0.0048192362477106</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>0.0102124989052883</v>
       </c>
-      <c r="J25">
+      <c r="M25">
         <v>0.0222169829713439</v>
       </c>
-      <c r="K25">
+      <c r="N25">
         <v>0.0328061328614695</v>
       </c>
-      <c r="L25" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="O25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C26">
+        <v>0.6156063675880432</v>
+      </c>
+      <c r="D26">
         <v>0.4328436851501465</v>
       </c>
-      <c r="D26">
-        <v>0.2099601427714029</v>
-      </c>
       <c r="E26">
-        <v>0.1276854217545059</v>
+        <v>0.5622794032096863</v>
       </c>
       <c r="F26">
         <v>0.4328436851501465</v>
       </c>
       <c r="G26">
-        <v>0.1259760856628418</v>
+        <v>0.2099601427714029</v>
       </c>
       <c r="H26">
-        <v>0.07022698223590849</v>
+        <v>0.1276854217545059</v>
       </c>
       <c r="I26">
         <v>0.4328436851501465</v>
       </c>
       <c r="J26">
+        <v>0.1259760856628418</v>
+      </c>
+      <c r="K26">
+        <v>0.07022698223590849</v>
+      </c>
+      <c r="L26">
+        <v>0.4328436851501465</v>
+      </c>
+      <c r="M26">
         <v>0.629880428314209</v>
       </c>
-      <c r="K26">
+      <c r="N26">
         <v>0.7022697925567627</v>
       </c>
-      <c r="L26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="O26" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>0.4126940667629242</v>
+        <v>0.5954087376594543</v>
       </c>
       <c r="D27">
-        <v>0.2004222828480932</v>
+        <v>0.4127486944198608</v>
       </c>
       <c r="E27">
-        <v>0.1227013764302592</v>
+        <v>0.5375679731369019</v>
       </c>
       <c r="F27">
         <v>0.4126940667629242</v>
       </c>
       <c r="G27">
-        <v>0.1202533692121505</v>
+        <v>0.200416223042541</v>
       </c>
       <c r="H27">
-        <v>0.0674857571721077</v>
+        <v>0.1227013764302592</v>
       </c>
       <c r="I27">
         <v>0.4126940667629242</v>
       </c>
       <c r="J27">
-        <v>0.6012668609619141</v>
+        <v>0.1202497333288192</v>
       </c>
       <c r="K27">
+        <v>0.0674857571721077</v>
+      </c>
+      <c r="L27">
+        <v>0.4126940667629242</v>
+      </c>
+      <c r="M27">
+        <v>0.6012486815452576</v>
+      </c>
+      <c r="N27">
         <v>0.6748575568199158</v>
       </c>
-      <c r="L27" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="O27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C28">
-        <v>0.3885764181613922</v>
+        <v>0.5732586979866028</v>
       </c>
       <c r="D28">
-        <v>0.1927653091649214</v>
+        <v>0.3882487714290619</v>
       </c>
       <c r="E28">
-        <v>0.1185149097245586</v>
+        <v>0.5134545564651489</v>
       </c>
       <c r="F28">
         <v>0.3885764181613922</v>
       </c>
       <c r="G28">
-        <v>0.1156591847538948</v>
+        <v>0.1927653091649214</v>
       </c>
       <c r="H28">
-        <v>0.0651831999421119</v>
+        <v>0.1185149097245586</v>
       </c>
       <c r="I28">
         <v>0.3885764181613922</v>
       </c>
       <c r="J28">
+        <v>0.1156591847538948</v>
+      </c>
+      <c r="K28">
+        <v>0.0651831999421119</v>
+      </c>
+      <c r="L28">
+        <v>0.3885764181613922</v>
+      </c>
+      <c r="M28">
         <v>0.5782959461212158</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>0.6518320441246033</v>
       </c>
-      <c r="L28" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="O28" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C29">
+        <v>0.1935119889844174</v>
+      </c>
+      <c r="D29">
+        <v>0.0313670157920442</v>
+      </c>
+      <c r="E29">
+        <v>0.0661783524168984</v>
+      </c>
+      <c r="F29">
         <v>0.0267383713479435</v>
       </c>
-      <c r="D29">
+      <c r="G29">
         <v>0.0299142905900771</v>
       </c>
-      <c r="E29">
+      <c r="H29">
         <v>0.0252819841435075</v>
       </c>
-      <c r="F29">
+      <c r="I29">
         <v>0.0313670157920442</v>
       </c>
-      <c r="G29">
+      <c r="J29">
         <v>0.019607098279699</v>
       </c>
-      <c r="H29">
+      <c r="K29">
         <v>0.0147365279209869</v>
       </c>
-      <c r="I29">
+      <c r="L29">
         <v>0.025017017655198</v>
       </c>
-      <c r="J29">
+      <c r="M29">
         <v>0.0757467085251078</v>
       </c>
-      <c r="K29">
+      <c r="N29">
         <v>0.1123620031191837</v>
       </c>
-      <c r="L29" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="O29" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C30">
+        <v>0.1812466704146589</v>
+      </c>
+      <c r="D30">
+        <v>0.0202149020459108</v>
+      </c>
+      <c r="E30">
+        <v>0.0510079603470087</v>
+      </c>
+      <c r="F30">
         <v>0.0172070155925368</v>
       </c>
-      <c r="D30">
+      <c r="G30">
         <v>0.0237329542543873</v>
       </c>
-      <c r="E30">
+      <c r="H30">
         <v>0.0201014522794471</v>
       </c>
-      <c r="F30">
+      <c r="I30">
         <v>0.0202149020459108</v>
       </c>
-      <c r="G30">
+      <c r="J30">
         <v>0.0154881423997393</v>
       </c>
-      <c r="H30">
+      <c r="K30">
         <v>0.011664948173876</v>
       </c>
-      <c r="I30">
+      <c r="L30">
         <v>0.0160921856986056</v>
       </c>
-      <c r="J30">
+      <c r="M30">
         <v>0.0605194359397109</v>
       </c>
-      <c r="K30">
+      <c r="N30">
         <v>0.0906054866242719</v>
       </c>
-      <c r="L30" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="O30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31">
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C31">
+        <v>0.1812554046721062</v>
+      </c>
+      <c r="D31">
+        <v>0.0202149020459108</v>
+      </c>
+      <c r="E31">
+        <v>0.0510131181469837</v>
+      </c>
+      <c r="F31">
         <v>0.0172070155925368</v>
       </c>
-      <c r="D31">
+      <c r="G31">
         <v>0.0237329542543873</v>
       </c>
-      <c r="E31">
+      <c r="H31">
         <v>0.0201014522794471</v>
       </c>
-      <c r="F31">
+      <c r="I31">
         <v>0.0202149020459108</v>
       </c>
-      <c r="G31">
+      <c r="J31">
         <v>0.0154881423997393</v>
       </c>
-      <c r="H31">
+      <c r="K31">
         <v>0.011664948173876</v>
       </c>
-      <c r="I31">
+      <c r="L31">
         <v>0.0160921856986056</v>
       </c>
-      <c r="J31">
+      <c r="M31">
         <v>0.0605194359397109</v>
       </c>
-      <c r="K31">
+      <c r="N31">
         <v>0.0906054866242719</v>
       </c>
-      <c r="L31" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="O31" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C32">
+        <v>0.8542130589485168</v>
+      </c>
+      <c r="D32">
         <v>0.7314998507499695</v>
       </c>
-      <c r="D32">
-        <v>0.3048984209696452</v>
-      </c>
       <c r="E32">
-        <v>0.1726647664692776</v>
+        <v>0.8429543375968933</v>
       </c>
       <c r="F32">
         <v>0.7314998507499695</v>
       </c>
       <c r="G32">
-        <v>0.1829390525817871</v>
+        <v>0.3048984209696452</v>
       </c>
       <c r="H32">
-        <v>0.0949656218290329</v>
+        <v>0.1726647664692776</v>
       </c>
       <c r="I32">
         <v>0.7314998507499695</v>
       </c>
       <c r="J32">
+        <v>0.1829390525817871</v>
+      </c>
+      <c r="K32">
+        <v>0.0949656218290329</v>
+      </c>
+      <c r="L32">
+        <v>0.7314998507499695</v>
+      </c>
+      <c r="M32">
         <v>0.9146952629089355</v>
       </c>
-      <c r="K32">
+      <c r="N32">
         <v>0.9496561884880066</v>
       </c>
-      <c r="L32" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" t="s">
+      <c r="O32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="P32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C33">
+        <v>0.8539680242538452</v>
+      </c>
+      <c r="D33">
         <v>0.7151846885681152</v>
       </c>
-      <c r="D33">
-        <v>0.3095598775479528</v>
-      </c>
       <c r="E33">
-        <v>0.1751438187173575</v>
+        <v>0.8454810976982117</v>
       </c>
       <c r="F33">
         <v>0.7151846885681152</v>
       </c>
       <c r="G33">
-        <v>0.1857359260320663</v>
+        <v>0.3095598775479528</v>
       </c>
       <c r="H33">
-        <v>0.09632910043001169</v>
+        <v>0.1751438187173575</v>
       </c>
       <c r="I33">
         <v>0.7151846885681152</v>
       </c>
       <c r="J33">
+        <v>0.1857359260320663</v>
+      </c>
+      <c r="K33">
+        <v>0.09632910043001169</v>
+      </c>
+      <c r="L33">
+        <v>0.7151846885681152</v>
+      </c>
+      <c r="M33">
         <v>0.9286796450614928</v>
       </c>
-      <c r="K33">
+      <c r="N33">
         <v>0.9632909893989564</v>
       </c>
-      <c r="L33" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" t="s">
+      <c r="O33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="P33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C34">
+        <v>0.8410143852233887</v>
+      </c>
+      <c r="D34">
         <v>0.7009672522544861</v>
       </c>
-      <c r="D34">
-        <v>0.303694208463033</v>
-      </c>
       <c r="E34">
-        <v>0.1725164459756583</v>
+        <v>0.8293303251266479</v>
       </c>
       <c r="F34">
         <v>0.7009672522544861</v>
       </c>
       <c r="G34">
-        <v>0.1822165250778198</v>
+        <v>0.303694208463033</v>
       </c>
       <c r="H34">
-        <v>0.0948840454220771</v>
+        <v>0.1725164459756583</v>
       </c>
       <c r="I34">
         <v>0.7009672522544861</v>
       </c>
       <c r="J34">
+        <v>0.1822165250778198</v>
+      </c>
+      <c r="K34">
+        <v>0.0948840454220771</v>
+      </c>
+      <c r="L34">
+        <v>0.7009672522544861</v>
+      </c>
+      <c r="M34">
         <v>0.9110826253890992</v>
       </c>
-      <c r="K34">
+      <c r="N34">
         <v>0.9488404393196106</v>
       </c>
-      <c r="L34" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="O34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="P34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C35">
+        <v>0.4993532225176924</v>
+      </c>
+      <c r="D35">
+        <v>0.217458148274684</v>
+      </c>
+      <c r="E35">
+        <v>0.4198549937563726</v>
+      </c>
+      <c r="F35">
         <v>0.1854276142754101</v>
       </c>
-      <c r="D35">
+      <c r="G35">
         <v>0.1936711439871704</v>
       </c>
-      <c r="E35">
+      <c r="H35">
         <v>0.1564264585110634</v>
       </c>
-      <c r="F35">
+      <c r="I35">
         <v>0.217458148274684</v>
       </c>
-      <c r="G35">
+      <c r="J35">
         <v>0.126819268875987</v>
       </c>
-      <c r="H35">
+      <c r="K35">
         <v>0.0911342671677553</v>
       </c>
-      <c r="I35">
+      <c r="L35">
         <v>0.1727341500317243</v>
       </c>
-      <c r="J35">
+      <c r="M35">
         <v>0.4826754600029282</v>
       </c>
-      <c r="K35">
+      <c r="N35">
         <v>0.6787080194792867</v>
       </c>
-      <c r="L35" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="O35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="P35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C36">
+        <v>0.485730962270092</v>
+      </c>
+      <c r="D36">
+        <v>0.2101127434233003</v>
+      </c>
+      <c r="E36">
+        <v>0.4006635549002124</v>
+      </c>
+      <c r="F36">
         <v>0.1791470084218628</v>
       </c>
-      <c r="D36">
+      <c r="G36">
         <v>0.1839695968155195</v>
       </c>
-      <c r="E36">
+      <c r="H36">
         <v>0.1516872831088455</v>
       </c>
-      <c r="F36">
+      <c r="I36">
         <v>0.2101127434233003</v>
       </c>
-      <c r="G36">
+      <c r="J36">
         <v>0.120567133583878</v>
       </c>
-      <c r="H36">
+      <c r="K36">
         <v>0.0883327639221109</v>
       </c>
-      <c r="I36">
+      <c r="L36">
         <v>0.1669688613402313</v>
       </c>
-      <c r="J36">
+      <c r="M36">
         <v>0.4576896952836482</v>
       </c>
-      <c r="K36">
+      <c r="N36">
         <v>0.6593406489118823</v>
       </c>
-      <c r="L36" t="s">
-        <v>20</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="O36" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="P36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37">
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C37">
+        <v>0.4857398850047244</v>
+      </c>
+      <c r="D37">
+        <v>0.2101127434233003</v>
+      </c>
+      <c r="E37">
+        <v>0.4006635549002124</v>
+      </c>
+      <c r="F37">
         <v>0.1791470084218628</v>
       </c>
-      <c r="D37">
+      <c r="G37">
         <v>0.1839695968155195</v>
       </c>
-      <c r="E37">
+      <c r="H37">
         <v>0.1516872831088455</v>
       </c>
-      <c r="F37">
+      <c r="I37">
         <v>0.2101127434233003</v>
       </c>
-      <c r="G37">
+      <c r="J37">
         <v>0.120567133583878</v>
       </c>
-      <c r="H37">
+      <c r="K37">
         <v>0.0883327639221109</v>
       </c>
-      <c r="I37">
+      <c r="L37">
         <v>0.1669688613402313</v>
       </c>
-      <c r="J37">
+      <c r="M37">
         <v>0.4576896952836482</v>
       </c>
-      <c r="K37">
+      <c r="N37">
         <v>0.6593406489118823</v>
       </c>
-      <c r="L37" t="s">
-        <v>20</v>
-      </c>
-      <c r="M37" t="s">
+      <c r="O37" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="P37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C38">
+        <v>0.8624147176742554</v>
+      </c>
+      <c r="D38">
         <v>0.7511768937110901</v>
       </c>
-      <c r="D38">
-        <v>0.3033792939451004</v>
-      </c>
       <c r="E38">
-        <v>0.1720975745807994</v>
+        <v>0.8510051965713501</v>
       </c>
       <c r="F38">
         <v>0.7511768937110901</v>
       </c>
       <c r="G38">
-        <v>0.1820275783538818</v>
+        <v>0.3033792939451004</v>
       </c>
       <c r="H38">
-        <v>0.0946536660194397</v>
+        <v>0.1720975745807994</v>
       </c>
       <c r="I38">
         <v>0.7511768937110901</v>
       </c>
       <c r="J38">
+        <v>0.1820275783538818</v>
+      </c>
+      <c r="K38">
+        <v>0.0946536660194397</v>
+      </c>
+      <c r="L38">
+        <v>0.7511768937110901</v>
+      </c>
+      <c r="M38">
         <v>0.9101378321647644</v>
       </c>
-      <c r="K38">
+      <c r="N38">
         <v>0.946536660194397</v>
       </c>
-      <c r="L38" t="s">
-        <v>20</v>
-      </c>
-      <c r="M38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="O38" t="s">
+        <v>23</v>
+      </c>
+      <c r="P38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39">
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C39">
+        <v>0.8629311323165894</v>
+      </c>
+      <c r="D39">
         <v>0.7372226119041443</v>
       </c>
-      <c r="D39">
-        <v>0.3094037133786413</v>
-      </c>
       <c r="E39">
-        <v>0.1753530586061399</v>
+        <v>0.8548914194107056</v>
       </c>
       <c r="F39">
         <v>0.7372226119041443</v>
       </c>
       <c r="G39">
-        <v>0.1856422275304794</v>
+        <v>0.3094037133786413</v>
       </c>
       <c r="H39">
-        <v>0.09644418209791179</v>
+        <v>0.1753530586061399</v>
       </c>
       <c r="I39">
         <v>0.7372226119041443</v>
       </c>
       <c r="J39">
+        <v>0.1856422275304794</v>
+      </c>
+      <c r="K39">
+        <v>0.09644418209791179</v>
+      </c>
+      <c r="L39">
+        <v>0.7372226119041443</v>
+      </c>
+      <c r="M39">
         <v>0.9282111525535583</v>
       </c>
-      <c r="K39">
+      <c r="N39">
         <v>0.9644418358802797</v>
       </c>
-      <c r="L39" t="s">
-        <v>20</v>
-      </c>
-      <c r="M39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="O39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C40">
-        <v>0.7051950097084045</v>
+        <v>0.8431017398834229</v>
       </c>
       <c r="D40">
-        <v>0.3029589851697286</v>
+        <v>0.7052791118621826</v>
       </c>
       <c r="E40">
-        <v>0.1726783671654945</v>
+        <v>0.8319594860076904</v>
       </c>
       <c r="F40">
         <v>0.7051950097084045</v>
       </c>
       <c r="G40">
-        <v>0.1817753911018371</v>
+        <v>0.3029589851697286</v>
       </c>
       <c r="H40">
-        <v>0.0949731022119522</v>
+        <v>0.1726783671654945</v>
       </c>
       <c r="I40">
         <v>0.7051950097084045</v>
       </c>
       <c r="J40">
+        <v>0.1817753911018371</v>
+      </c>
+      <c r="K40">
+        <v>0.0949731022119522</v>
+      </c>
+      <c r="L40">
+        <v>0.7051950097084045</v>
+      </c>
+      <c r="M40">
         <v>0.9088769555091858</v>
       </c>
-      <c r="K40">
+      <c r="N40">
         <v>0.9497309923171996</v>
       </c>
-      <c r="L40" t="s">
-        <v>20</v>
-      </c>
-      <c r="M40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="O40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41">
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C41">
+        <v>0.4768527083255887</v>
+      </c>
+      <c r="D41">
+        <v>0.2098954348380515</v>
+      </c>
+      <c r="E41">
+        <v>0.3876693536867969</v>
+      </c>
+      <c r="F41">
         <v>0.1773605459196269</v>
       </c>
-      <c r="D41">
+      <c r="G41">
         <v>0.1782121343842211</v>
       </c>
-      <c r="E41">
+      <c r="H41">
         <v>0.1439460859866758</v>
       </c>
-      <c r="F41">
+      <c r="I41">
         <v>0.2098954348380515</v>
       </c>
-      <c r="G41">
+      <c r="J41">
         <v>0.117648559041069</v>
       </c>
-      <c r="H41">
+      <c r="K41">
         <v>0.08448099974497129</v>
       </c>
-      <c r="I41">
+      <c r="L41">
         <v>0.1648306506793109</v>
       </c>
-      <c r="J41">
+      <c r="M41">
         <v>0.441719563922512</v>
       </c>
-      <c r="K41">
+      <c r="N41">
         <v>0.6187086019112927</v>
       </c>
-      <c r="L41" t="s">
-        <v>20</v>
-      </c>
-      <c r="M41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="O41" t="s">
+        <v>23</v>
+      </c>
+      <c r="P41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42">
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C42">
+        <v>0.4518580067190288</v>
+      </c>
+      <c r="D42">
+        <v>0.1648814078041316</v>
+      </c>
+      <c r="E42">
+        <v>0.355196980255674</v>
+      </c>
+      <c r="F42">
         <v>0.137318914791538</v>
       </c>
-      <c r="D42">
+      <c r="G42">
         <v>0.1660272184960325</v>
       </c>
-      <c r="E42">
+      <c r="H42">
         <v>0.1370988691309279</v>
       </c>
-      <c r="F42">
+      <c r="I42">
         <v>0.1648814078041316</v>
       </c>
-      <c r="G42">
+      <c r="J42">
         <v>0.1098444274419856</v>
       </c>
-      <c r="H42">
+      <c r="K42">
         <v>0.0805406783983752</v>
       </c>
-      <c r="I42">
+      <c r="L42">
         <v>0.1269423265151643</v>
       </c>
-      <c r="J42">
+      <c r="M42">
         <v>0.4106367813864627</v>
       </c>
-      <c r="K42">
+      <c r="N42">
         <v>0.5893421669298495</v>
       </c>
-      <c r="L42" t="s">
-        <v>20</v>
-      </c>
-      <c r="M42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="O42" t="s">
+        <v>23</v>
+      </c>
+      <c r="P42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43">
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C43">
+        <v>0.4518702347680352</v>
+      </c>
+      <c r="D43">
+        <v>0.1648814078041316</v>
+      </c>
+      <c r="E43">
+        <v>0.355196980255674</v>
+      </c>
+      <c r="F43">
         <v>0.137318914791538</v>
       </c>
-      <c r="D43">
+      <c r="G43">
         <v>0.1660272184960325</v>
       </c>
-      <c r="E43">
+      <c r="H43">
         <v>0.1370988691309279</v>
       </c>
-      <c r="F43">
+      <c r="I43">
         <v>0.1648814078041316</v>
       </c>
-      <c r="G43">
+      <c r="J43">
         <v>0.1098444274419856</v>
       </c>
-      <c r="H43">
+      <c r="K43">
         <v>0.0805406783983752</v>
       </c>
-      <c r="I43">
+      <c r="L43">
         <v>0.1269423265151643</v>
       </c>
-      <c r="J43">
+      <c r="M43">
         <v>0.4106367813864627</v>
       </c>
-      <c r="K43">
+      <c r="N43">
         <v>0.5893421669298495</v>
       </c>
-      <c r="L43" t="s">
-        <v>20</v>
-      </c>
-      <c r="M43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="O43" t="s">
+        <v>23</v>
+      </c>
+      <c r="P43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C44">
+        <v>0.8979824781417847</v>
+      </c>
+      <c r="D44">
         <v>0.7991133332252502</v>
       </c>
-      <c r="D44">
-        <v>0.3172624078061843</v>
-      </c>
       <c r="E44">
-        <v>0.1772840599383204</v>
+        <v>0.8921695947647095</v>
       </c>
       <c r="F44">
         <v>0.7991133332252502</v>
       </c>
       <c r="G44">
-        <v>0.1903574466705322</v>
+        <v>0.3172624078061843</v>
       </c>
       <c r="H44">
-        <v>0.0975062325596809</v>
+        <v>0.1772840599383204</v>
       </c>
       <c r="I44">
         <v>0.7991133332252502</v>
       </c>
       <c r="J44">
+        <v>0.1903574466705322</v>
+      </c>
+      <c r="K44">
+        <v>0.0975062325596809</v>
+      </c>
+      <c r="L44">
+        <v>0.7991133332252502</v>
+      </c>
+      <c r="M44">
         <v>0.9517871737480164</v>
       </c>
-      <c r="K44">
+      <c r="N44">
         <v>0.975062370300293</v>
       </c>
-      <c r="L44" t="s">
-        <v>20</v>
-      </c>
-      <c r="M44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="O44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45">
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C45">
+        <v>0.8891003131866455</v>
+      </c>
+      <c r="D45">
         <v>0.7793017625808716</v>
       </c>
-      <c r="D45">
-        <v>0.3165696817967626</v>
-      </c>
       <c r="E45">
-        <v>0.177510773347429</v>
+        <v>0.8833838105201721</v>
       </c>
       <c r="F45">
         <v>0.7793017625808716</v>
       </c>
       <c r="G45">
-        <v>0.1899418085813522</v>
+        <v>0.3165696817967626</v>
       </c>
       <c r="H45">
-        <v>0.097630925476551</v>
+        <v>0.177510773347429</v>
       </c>
       <c r="I45">
         <v>0.7793017625808716</v>
       </c>
       <c r="J45">
+        <v>0.1899418085813522</v>
+      </c>
+      <c r="K45">
+        <v>0.097630925476551</v>
+      </c>
+      <c r="L45">
+        <v>0.7793017625808716</v>
+      </c>
+      <c r="M45">
         <v>0.9497090578079224</v>
       </c>
-      <c r="K45">
+      <c r="N45">
         <v>0.9763092398643494</v>
       </c>
-      <c r="L45" t="s">
-        <v>20</v>
-      </c>
-      <c r="M45" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="O45" t="s">
+        <v>23</v>
+      </c>
+      <c r="P45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46">
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C46">
+        <v>0.8725389838218689</v>
+      </c>
+      <c r="D46">
         <v>0.7492380142211914</v>
       </c>
-      <c r="D46">
-        <v>0.3125057650936972</v>
-      </c>
       <c r="E46">
-        <v>0.1765031839205214</v>
+        <v>0.8657087087631226</v>
       </c>
       <c r="F46">
         <v>0.7492380142211914</v>
       </c>
       <c r="G46">
-        <v>0.1875034570693969</v>
+        <v>0.3125057650936972</v>
       </c>
       <c r="H46">
-        <v>0.09707675129175181</v>
+        <v>0.1765031839205214</v>
       </c>
       <c r="I46">
         <v>0.7492380142211914</v>
       </c>
       <c r="J46">
+        <v>0.1875034570693969</v>
+      </c>
+      <c r="K46">
+        <v>0.09707675129175181</v>
+      </c>
+      <c r="L46">
+        <v>0.7492380142211914</v>
+      </c>
+      <c r="M46">
         <v>0.9375173449516296</v>
       </c>
-      <c r="K46">
+      <c r="N46">
         <v>0.9707674980163574</v>
       </c>
-      <c r="L46" t="s">
-        <v>20</v>
-      </c>
-      <c r="M46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="O46" t="s">
+        <v>23</v>
+      </c>
+      <c r="P46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47">
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C47">
+        <v>0.5629256362924275</v>
+      </c>
+      <c r="D47">
+        <v>0.2873900293255132</v>
+      </c>
+      <c r="E47">
+        <v>0.5009769441437498</v>
+      </c>
+      <c r="F47">
         <v>0.2385864903146002</v>
       </c>
-      <c r="D47">
+      <c r="G47">
         <v>0.234869174720456</v>
       </c>
-      <c r="E47">
+      <c r="H47">
         <v>0.1857657986718306</v>
       </c>
-      <c r="F47">
+      <c r="I47">
         <v>0.2873900293255132</v>
       </c>
-      <c r="G47">
+      <c r="J47">
         <v>0.1566401340594949</v>
       </c>
-      <c r="H47">
+      <c r="K47">
         <v>0.1095098449937229</v>
       </c>
-      <c r="I47">
+      <c r="L47">
         <v>0.2194823481689841</v>
       </c>
-      <c r="J47">
+      <c r="M47">
         <v>0.5618825002675027</v>
       </c>
-      <c r="K47">
+      <c r="N47">
         <v>0.764889786004155</v>
       </c>
-      <c r="L47" t="s">
-        <v>20</v>
-      </c>
-      <c r="M47" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="O47" t="s">
+        <v>23</v>
+      </c>
+      <c r="P47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48">
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C48">
+        <v>0.5315172157290358</v>
+      </c>
+      <c r="D48">
+        <v>0.23292836196062</v>
+      </c>
+      <c r="E48">
+        <v>0.4644986984113075</v>
+      </c>
+      <c r="F48">
         <v>0.1916302591417795</v>
       </c>
-      <c r="D48">
+      <c r="G48">
         <v>0.2209408330114308</v>
       </c>
-      <c r="E48">
+      <c r="H48">
         <v>0.1810943686495428</v>
       </c>
-      <c r="F48">
+      <c r="I48">
         <v>0.23292836196062</v>
       </c>
-      <c r="G48">
+      <c r="J48">
         <v>0.1472559698366194</v>
       </c>
-      <c r="H48">
+      <c r="K48">
         <v>0.1067029744449164</v>
       </c>
-      <c r="I48">
+      <c r="L48">
         <v>0.1757013095827506</v>
       </c>
-      <c r="J48">
+      <c r="M48">
         <v>0.5293763084190399</v>
       </c>
-      <c r="K48">
+      <c r="N48">
         <v>0.7468564996424231</v>
       </c>
-      <c r="L48" t="s">
-        <v>20</v>
-      </c>
-      <c r="M48" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="O48" t="s">
+        <v>23</v>
+      </c>
+      <c r="P48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49">
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C49">
+        <v>0.531524181448166</v>
+      </c>
+      <c r="D49">
+        <v>0.23292836196062</v>
+      </c>
+      <c r="E49">
+        <v>0.4644986984113075</v>
+      </c>
+      <c r="F49">
         <v>0.1916302591417795</v>
       </c>
-      <c r="D49">
+      <c r="G49">
         <v>0.2209408330114308</v>
       </c>
-      <c r="E49">
+      <c r="H49">
         <v>0.1810943686495428</v>
       </c>
-      <c r="F49">
+      <c r="I49">
         <v>0.23292836196062</v>
       </c>
-      <c r="G49">
+      <c r="J49">
         <v>0.1472559698366194</v>
       </c>
-      <c r="H49">
+      <c r="K49">
         <v>0.1067029744449164</v>
       </c>
-      <c r="I49">
+      <c r="L49">
         <v>0.1757013095827506</v>
       </c>
-      <c r="J49">
+      <c r="M49">
         <v>0.5293763084190399</v>
       </c>
-      <c r="K49">
+      <c r="N49">
         <v>0.7468564996424231</v>
       </c>
-      <c r="L49" t="s">
-        <v>20</v>
-      </c>
-      <c r="M49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="O49" t="s">
+        <v>23</v>
+      </c>
+      <c r="P49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50">
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C50">
+        <v>0.8859732151031494</v>
+      </c>
+      <c r="D50">
         <v>0.7731395959854126</v>
       </c>
-      <c r="D50">
-        <v>0.3163334487213028</v>
-      </c>
       <c r="E50">
-        <v>0.1766012606541972</v>
+        <v>0.8794039487838745</v>
       </c>
       <c r="F50">
         <v>0.7731395959854126</v>
       </c>
       <c r="G50">
-        <v>0.1898000687360763</v>
+        <v>0.3163334487213028</v>
       </c>
       <c r="H50">
-        <v>0.09713069349527351</v>
+        <v>0.1766012606541972</v>
       </c>
       <c r="I50">
         <v>0.7731395959854126</v>
       </c>
       <c r="J50">
+        <v>0.1898000687360763</v>
+      </c>
+      <c r="K50">
+        <v>0.09713069349527351</v>
+      </c>
+      <c r="L50">
+        <v>0.7731395959854126</v>
+      </c>
+      <c r="M50">
         <v>0.949000358581543</v>
       </c>
-      <c r="K50">
+      <c r="N50">
         <v>0.9713069200515748</v>
       </c>
-      <c r="L50" t="s">
-        <v>20</v>
-      </c>
-      <c r="M50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="O50" t="s">
+        <v>23</v>
+      </c>
+      <c r="P50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51">
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C51">
+        <v>0.8823725581169128</v>
+      </c>
+      <c r="D51">
         <v>0.7629581689834595</v>
       </c>
-      <c r="D51">
-        <v>0.3164568783508407</v>
-      </c>
       <c r="E51">
-        <v>0.177122950553894</v>
+        <v>0.8762820959091187</v>
       </c>
       <c r="F51">
         <v>0.7629581689834595</v>
       </c>
       <c r="G51">
-        <v>0.1898741275072097</v>
+        <v>0.3164568783508407</v>
       </c>
       <c r="H51">
-        <v>0.0974176228046417</v>
+        <v>0.177122950553894</v>
       </c>
       <c r="I51">
         <v>0.7629581689834595</v>
       </c>
       <c r="J51">
+        <v>0.1898741275072097</v>
+      </c>
+      <c r="K51">
+        <v>0.0974176228046417</v>
+      </c>
+      <c r="L51">
+        <v>0.7629581689834595</v>
+      </c>
+      <c r="M51">
         <v>0.9493706226348876</v>
       </c>
-      <c r="K51">
+      <c r="N51">
         <v>0.9741762280464172</v>
       </c>
-      <c r="L51" t="s">
-        <v>20</v>
-      </c>
-      <c r="M51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="O51" t="s">
+        <v>23</v>
+      </c>
+      <c r="P51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C52">
-        <v>0.7159385681152344</v>
+        <v>0.8549696207046509</v>
       </c>
       <c r="D52">
-        <v>0.3089596347676382</v>
+        <v>0.7160310745239258</v>
       </c>
       <c r="E52">
-        <v>0.1750866667298246</v>
+        <v>0.8464776873588562</v>
       </c>
       <c r="F52">
         <v>0.7159385681152344</v>
       </c>
       <c r="G52">
-        <v>0.1853757798671722</v>
+        <v>0.3089596347676382</v>
       </c>
       <c r="H52">
-        <v>0.0962976664304733</v>
+        <v>0.1750866667298246</v>
       </c>
       <c r="I52">
         <v>0.7159385681152344</v>
       </c>
       <c r="J52">
+        <v>0.1853757798671722</v>
+      </c>
+      <c r="K52">
+        <v>0.0962976664304733</v>
+      </c>
+      <c r="L52">
+        <v>0.7159385681152344</v>
+      </c>
+      <c r="M52">
         <v>0.9268789291381836</v>
       </c>
-      <c r="K52">
+      <c r="N52">
         <v>0.9629766941070556</v>
       </c>
-      <c r="L52" t="s">
-        <v>20</v>
-      </c>
-      <c r="M52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="O52" t="s">
+        <v>23</v>
+      </c>
+      <c r="P52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53">
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C53">
+        <v>0.4932079309079208</v>
+      </c>
+      <c r="D53">
+        <v>0.2127289955780164</v>
+      </c>
+      <c r="E53">
+        <v>0.3964155113076378</v>
+      </c>
+      <c r="F53">
         <v>0.1651162479401854</v>
       </c>
-      <c r="D53">
+      <c r="G53">
         <v>0.1913287713323017</v>
       </c>
-      <c r="E53">
+      <c r="H53">
         <v>0.1654914718402866</v>
       </c>
-      <c r="F53">
+      <c r="I53">
         <v>0.2127289955780164</v>
       </c>
-      <c r="G53">
+      <c r="J53">
         <v>0.1320593809223065</v>
       </c>
-      <c r="H53">
+      <c r="K53">
         <v>0.0997946936197176</v>
       </c>
-      <c r="I53">
+      <c r="L53">
         <v>0.1482323032919212</v>
       </c>
-      <c r="J53">
+      <c r="M53">
         <v>0.4324531668321145</v>
       </c>
-      <c r="K53">
+      <c r="N53">
         <v>0.6358960595714381</v>
       </c>
-      <c r="L53" t="s">
-        <v>20</v>
-      </c>
-      <c r="M53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="O53" t="s">
+        <v>23</v>
+      </c>
+      <c r="P53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54">
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C54">
+        <v>0.4751515399322715</v>
+      </c>
+      <c r="D54">
+        <v>0.1942514213518635</v>
+      </c>
+      <c r="E54">
+        <v>0.3741198733342352</v>
+      </c>
+      <c r="F54">
         <v>0.1481653109008089</v>
       </c>
-      <c r="D54">
+      <c r="G54">
         <v>0.1781801534379506</v>
       </c>
-      <c r="E54">
+      <c r="H54">
         <v>0.1612027472199091</v>
       </c>
-      <c r="F54">
+      <c r="I54">
         <v>0.1942514213518635</v>
       </c>
-      <c r="G54">
+      <c r="J54">
         <v>0.1229943145925513</v>
       </c>
-      <c r="H54">
+      <c r="K54">
         <v>0.09722046746684269</v>
       </c>
-      <c r="I54">
+      <c r="L54">
         <v>0.1320236277812873</v>
       </c>
-      <c r="J54">
+      <c r="M54">
         <v>0.4048551574767617</v>
       </c>
-      <c r="K54">
+      <c r="N54">
         <v>0.6198731061175783</v>
       </c>
-      <c r="L54" t="s">
-        <v>20</v>
-      </c>
-      <c r="M54" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="O54" t="s">
+        <v>23</v>
+      </c>
+      <c r="P54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55">
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C55">
+        <v>0.4751586884114687</v>
+      </c>
+      <c r="D55">
+        <v>0.1942514213518635</v>
+      </c>
+      <c r="E55">
+        <v>0.3741198733342352</v>
+      </c>
+      <c r="F55">
         <v>0.1481653109008089</v>
       </c>
-      <c r="D55">
+      <c r="G55">
         <v>0.1781801534379506</v>
       </c>
-      <c r="E55">
+      <c r="H55">
         <v>0.1612027472199091</v>
       </c>
-      <c r="F55">
+      <c r="I55">
         <v>0.1942514213518635</v>
       </c>
-      <c r="G55">
+      <c r="J55">
         <v>0.1229943145925513</v>
       </c>
-      <c r="H55">
+      <c r="K55">
         <v>0.09722046746684269</v>
       </c>
-      <c r="I55">
+      <c r="L55">
         <v>0.1320236277812873</v>
       </c>
-      <c r="J55">
+      <c r="M55">
         <v>0.4048551574767617</v>
       </c>
-      <c r="K55">
+      <c r="N55">
         <v>0.6198731061175783</v>
       </c>
-      <c r="L55" t="s">
-        <v>20</v>
-      </c>
-      <c r="M55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="O55" t="s">
+        <v>23</v>
+      </c>
+      <c r="P55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C56">
+        <v>0.8807642459869385</v>
+      </c>
+      <c r="D56">
         <v>0.7658023834228516</v>
       </c>
-      <c r="D56">
-        <v>0.3142405276497204</v>
-      </c>
       <c r="E56">
-        <v>0.1777818803944863</v>
+        <v>0.8754671812057495</v>
       </c>
       <c r="F56">
         <v>0.7658023834228516</v>
       </c>
       <c r="G56">
-        <v>0.1885443180799484</v>
+        <v>0.3142405276497204</v>
       </c>
       <c r="H56">
-        <v>0.0977800339460372</v>
+        <v>0.1777818803944863</v>
       </c>
       <c r="I56">
         <v>0.7658023834228516</v>
       </c>
       <c r="J56">
+        <v>0.1885443180799484</v>
+      </c>
+      <c r="K56">
+        <v>0.0977800339460372</v>
+      </c>
+      <c r="L56">
+        <v>0.7658023834228516</v>
+      </c>
+      <c r="M56">
         <v>0.9427215456962584</v>
       </c>
-      <c r="K56">
+      <c r="N56">
         <v>0.9778003692626952</v>
       </c>
-      <c r="L56" t="s">
-        <v>20</v>
-      </c>
-      <c r="M56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="O56" t="s">
+        <v>23</v>
+      </c>
+      <c r="P56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57">
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C57">
+        <v>0.8800721168518066</v>
+      </c>
+      <c r="D57">
         <v>0.7656329274177551</v>
       </c>
-      <c r="D57">
-        <v>0.3143535057703654</v>
-      </c>
       <c r="E57">
-        <v>0.1765186136419123</v>
+        <v>0.8733294606208801</v>
       </c>
       <c r="F57">
         <v>0.7656329274177551</v>
       </c>
       <c r="G57">
-        <v>0.1886121034622192</v>
+        <v>0.3143535057703654</v>
       </c>
       <c r="H57">
-        <v>0.0970852375030517</v>
+        <v>0.1765186136419123</v>
       </c>
       <c r="I57">
         <v>0.7656329274177551</v>
       </c>
       <c r="J57">
+        <v>0.1886121034622192</v>
+      </c>
+      <c r="K57">
+        <v>0.0970852375030517</v>
+      </c>
+      <c r="L57">
+        <v>0.7656329274177551</v>
+      </c>
+      <c r="M57">
         <v>0.9430605173110962</v>
       </c>
-      <c r="K57">
+      <c r="N57">
         <v>0.9708523750305176</v>
       </c>
-      <c r="L57" t="s">
-        <v>20</v>
-      </c>
-      <c r="M57" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="O57" t="s">
+        <v>23</v>
+      </c>
+      <c r="P57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58">
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C58">
+        <v>0.8585981726646423</v>
+      </c>
+      <c r="D58">
         <v>0.7230978012084961</v>
       </c>
-      <c r="D58">
-        <v>0.3103428838981522</v>
-      </c>
       <c r="E58">
-        <v>0.1755018401737055</v>
+        <v>0.8505347967147827</v>
       </c>
       <c r="F58">
         <v>0.7230978012084961</v>
       </c>
       <c r="G58">
-        <v>0.1862057298421859</v>
+        <v>0.3103428838981522</v>
       </c>
       <c r="H58">
-        <v>0.09652601182460779</v>
+        <v>0.1755018401737055</v>
       </c>
       <c r="I58">
         <v>0.7230978012084961</v>
       </c>
       <c r="J58">
+        <v>0.1862057298421859</v>
+      </c>
+      <c r="K58">
+        <v>0.09652601182460779</v>
+      </c>
+      <c r="L58">
+        <v>0.7230978012084961</v>
+      </c>
+      <c r="M58">
         <v>0.9310286641120912</v>
       </c>
-      <c r="K58">
+      <c r="N58">
         <v>0.9652601480484008</v>
       </c>
-      <c r="L58" t="s">
-        <v>20</v>
-      </c>
-      <c r="M58" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="O58" t="s">
+        <v>23</v>
+      </c>
+      <c r="P58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59">
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C59">
+        <v>0.470173614100276</v>
+      </c>
+      <c r="D59">
+        <v>0.1821903787103377</v>
+      </c>
+      <c r="E59">
+        <v>0.3789146807346903</v>
+      </c>
+      <c r="F59">
         <v>0.14967141070007</v>
       </c>
-      <c r="D59">
+      <c r="G59">
         <v>0.1756430682562625</v>
       </c>
-      <c r="E59">
+      <c r="H59">
         <v>0.1541800125019273</v>
       </c>
-      <c r="F59">
+      <c r="I59">
         <v>0.1821903787103377</v>
       </c>
-      <c r="G59">
+      <c r="J59">
         <v>0.117093142272258</v>
       </c>
-      <c r="H59">
+      <c r="K59">
         <v>0.0906090071647928</v>
       </c>
-      <c r="I59">
+      <c r="L59">
         <v>0.1369498464687819</v>
       </c>
-      <c r="J59">
+      <c r="M59">
         <v>0.4209305088463227</v>
       </c>
-      <c r="K59">
+      <c r="N59">
         <v>0.6416727591753182</v>
       </c>
-      <c r="L59" t="s">
-        <v>20</v>
-      </c>
-      <c r="M59" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="O59" t="s">
+        <v>23</v>
+      </c>
+      <c r="P59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60">
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C60">
+        <v>0.4555109516644589</v>
+      </c>
+      <c r="D60">
+        <v>0.1627430910951893</v>
+      </c>
+      <c r="E60">
+        <v>0.3573750139669672</v>
+      </c>
+      <c r="F60">
         <v>0.1337419375802181</v>
       </c>
-      <c r="D60">
+      <c r="G60">
         <v>0.164658275157855</v>
       </c>
-      <c r="E60">
+      <c r="H60">
         <v>0.1479649128525466</v>
       </c>
-      <c r="F60">
+      <c r="I60">
         <v>0.1627430910951893</v>
       </c>
-      <c r="G60">
+      <c r="J60">
         <v>0.1099283520982564</v>
       </c>
-      <c r="H60">
+      <c r="K60">
         <v>0.0869498464687842</v>
       </c>
-      <c r="I60">
+      <c r="L60">
         <v>0.1224709996588194</v>
       </c>
-      <c r="J60">
+      <c r="M60">
         <v>0.3932156869912755</v>
       </c>
-      <c r="K60">
+      <c r="N60">
         <v>0.6168494419262075</v>
       </c>
-      <c r="L60" t="s">
-        <v>20</v>
-      </c>
-      <c r="M60" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="O60" t="s">
+        <v>23</v>
+      </c>
+      <c r="P60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61">
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C61">
+        <v>0.4555125377664709</v>
+      </c>
+      <c r="D61">
+        <v>0.1627430910951893</v>
+      </c>
+      <c r="E61">
+        <v>0.3573750139669672</v>
+      </c>
+      <c r="F61">
         <v>0.1337419375802181</v>
       </c>
-      <c r="D61">
+      <c r="G61">
         <v>0.164658275157855</v>
       </c>
-      <c r="E61">
+      <c r="H61">
         <v>0.1479649128525466</v>
       </c>
-      <c r="F61">
+      <c r="I61">
         <v>0.1627430910951893</v>
       </c>
-      <c r="G61">
+      <c r="J61">
         <v>0.1099283520982564</v>
       </c>
-      <c r="H61">
+      <c r="K61">
         <v>0.0869498464687842</v>
       </c>
-      <c r="I61">
+      <c r="L61">
         <v>0.1224709996588194</v>
       </c>
-      <c r="J61">
+      <c r="M61">
         <v>0.3932156869912755</v>
       </c>
-      <c r="K61">
+      <c r="N61">
         <v>0.6168494419262075</v>
       </c>
-      <c r="L61" t="s">
-        <v>20</v>
-      </c>
-      <c r="M61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="O61" t="s">
+        <v>23</v>
+      </c>
+      <c r="P61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62">
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C62">
+        <v>0.7129588476703855</v>
+      </c>
+      <c r="D62">
+        <v>0.6210032267527134</v>
+      </c>
+      <c r="E62">
+        <v>0.6739866700298976</v>
+      </c>
+      <c r="F62">
         <v>0.6107362863009685</v>
       </c>
-      <c r="D62">
+      <c r="G62">
         <v>0.2436233220187529</v>
       </c>
-      <c r="E62">
+      <c r="H62">
         <v>0.1360077294368905</v>
       </c>
-      <c r="F62">
+      <c r="I62">
         <v>0.6210032267527134</v>
       </c>
-      <c r="G62">
+      <c r="J62">
         <v>0.1482546201231975</v>
       </c>
-      <c r="H62">
+      <c r="K62">
         <v>0.07544734526253739</v>
       </c>
-      <c r="I62">
+      <c r="L62">
         <v>0.6058570450767576</v>
       </c>
-      <c r="J62">
+      <c r="M62">
         <v>0.7076366480883935</v>
       </c>
-      <c r="K62">
+      <c r="N62">
         <v>0.7194680747042145</v>
       </c>
-      <c r="L62" t="s">
-        <v>21</v>
-      </c>
-      <c r="M62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="O62" t="s">
+        <v>24</v>
+      </c>
+      <c r="P62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63">
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C63">
+        <v>0.5967362523078918</v>
+      </c>
+      <c r="D63">
         <v>0.2937880754470825</v>
       </c>
-      <c r="D63">
-        <v>0.2354851845237943</v>
-      </c>
       <c r="E63">
-        <v>0.1439043332722561</v>
+        <v>0.5570669770240784</v>
       </c>
       <c r="F63">
         <v>0.2937880754470825</v>
       </c>
       <c r="G63">
-        <v>0.1412911117076873</v>
+        <v>0.2354851845237943</v>
       </c>
       <c r="H63">
-        <v>0.079147383570671</v>
+        <v>0.1439043332722561</v>
       </c>
       <c r="I63">
         <v>0.2937880754470825</v>
       </c>
       <c r="J63">
+        <v>0.1412911117076873</v>
+      </c>
+      <c r="K63">
+        <v>0.079147383570671</v>
+      </c>
+      <c r="L63">
+        <v>0.2937880754470825</v>
+      </c>
+      <c r="M63">
         <v>0.7064555287361145</v>
       </c>
-      <c r="K63">
+      <c r="N63">
         <v>0.7914738059043884</v>
       </c>
-      <c r="L63" t="s">
-        <v>21</v>
-      </c>
-      <c r="M63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="O63" t="s">
+        <v>24</v>
+      </c>
+      <c r="P63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64">
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C64">
-        <v>0.2294762432575225</v>
+        <v>0.5321927070617676</v>
       </c>
       <c r="D64">
-        <v>0.2061713358594311</v>
+        <v>0.2302070707082748</v>
       </c>
       <c r="E64">
-        <v>0.1292437181985082</v>
+        <v>0.4795117378234863</v>
       </c>
       <c r="F64">
         <v>0.2294762432575225</v>
       </c>
       <c r="G64">
-        <v>0.1237028017640113</v>
+        <v>0.2061713358594311</v>
       </c>
       <c r="H64">
-        <v>0.07108404487371441</v>
+        <v>0.1292437181985082</v>
       </c>
       <c r="I64">
         <v>0.2294762432575225</v>
       </c>
       <c r="J64">
+        <v>0.1237028017640113</v>
+      </c>
+      <c r="K64">
+        <v>0.07108404487371441</v>
+      </c>
+      <c r="L64">
+        <v>0.2294762432575225</v>
+      </c>
+      <c r="M64">
         <v>0.6185140013694763</v>
       </c>
-      <c r="K64">
+      <c r="N64">
         <v>0.7108404636383057</v>
       </c>
-      <c r="L64" t="s">
-        <v>21</v>
-      </c>
-      <c r="M64" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="O64" t="s">
+        <v>24</v>
+      </c>
+      <c r="P64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65">
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C65">
+        <v>0.3026963482068906</v>
+      </c>
+      <c r="D65">
+        <v>0.09064241713112341</v>
+      </c>
+      <c r="E65">
+        <v>0.1846579398262904</v>
+      </c>
+      <c r="F65">
         <v>0.0899579544343404</v>
       </c>
-      <c r="D65">
+      <c r="G65">
         <v>0.0703075891547591</v>
       </c>
-      <c r="E65">
+      <c r="H65">
         <v>0.0523131898901928</v>
       </c>
-      <c r="F65">
+      <c r="I65">
         <v>0.09064241713112341</v>
       </c>
-      <c r="G65">
+      <c r="J65">
         <v>0.0423584628923438</v>
       </c>
-      <c r="H65">
+      <c r="K65">
         <v>0.0288354356116159</v>
       </c>
-      <c r="I65">
+      <c r="L65">
         <v>0.0896157230859489</v>
       </c>
-      <c r="J65">
+      <c r="M65">
         <v>0.20881001271145</v>
       </c>
-      <c r="K65">
+      <c r="N65">
         <v>0.2846387014764838</v>
       </c>
-      <c r="L65" t="s">
-        <v>21</v>
-      </c>
-      <c r="M65" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="O65" t="s">
+        <v>24</v>
+      </c>
+      <c r="P65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66">
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C66">
+        <v>0.301997334389695</v>
+      </c>
+      <c r="D66">
+        <v>0.0894690525080668</v>
+      </c>
+      <c r="E66">
+        <v>0.1841830038196574</v>
+      </c>
+      <c r="F66">
         <v>0.08868680942602911</v>
       </c>
-      <c r="D66">
+      <c r="G66">
         <v>0.0703075891547591</v>
       </c>
-      <c r="E66">
+      <c r="H66">
         <v>0.0523131898901928</v>
       </c>
-      <c r="F66">
+      <c r="I66">
         <v>0.0894690525080668</v>
       </c>
-      <c r="G66">
+      <c r="J66">
         <v>0.0423584628923438</v>
       </c>
-      <c r="H66">
+      <c r="K66">
         <v>0.0288354356116159</v>
       </c>
-      <c r="I66">
+      <c r="L66">
         <v>0.0882956878850102</v>
       </c>
-      <c r="J66">
+      <c r="M66">
         <v>0.20881001271145</v>
       </c>
-      <c r="K66">
+      <c r="N66">
         <v>0.2846387014764838</v>
       </c>
-      <c r="L66" t="s">
-        <v>21</v>
-      </c>
-      <c r="M66" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="O66" t="s">
+        <v>24</v>
+      </c>
+      <c r="P66" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67">
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C67">
+        <v>0.2964783906936645</v>
+      </c>
+      <c r="D67">
         <v>0.07844092696905131</v>
       </c>
-      <c r="D67">
-        <v>0.06252537771231589</v>
-      </c>
       <c r="E67">
-        <v>0.0600597942171017</v>
+        <v>0.1880343109369278</v>
       </c>
       <c r="F67">
         <v>0.07844092696905131</v>
       </c>
       <c r="G67">
-        <v>0.0375152267515659</v>
+        <v>0.06252537771231589</v>
       </c>
       <c r="H67">
-        <v>0.0330328866839408</v>
+        <v>0.0600597942171017</v>
       </c>
       <c r="I67">
         <v>0.07844092696905131</v>
       </c>
       <c r="J67">
+        <v>0.0375152267515659</v>
+      </c>
+      <c r="K67">
+        <v>0.0330328866839408</v>
+      </c>
+      <c r="L67">
+        <v>0.07844092696905131</v>
+      </c>
+      <c r="M67">
         <v>0.1875761300325393</v>
       </c>
-      <c r="K67">
+      <c r="N67">
         <v>0.33032888174057</v>
       </c>
-      <c r="L67" t="s">
-        <v>21</v>
-      </c>
-      <c r="M67" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="O67" t="s">
+        <v>24</v>
+      </c>
+      <c r="P67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68">
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C68">
-        <v>0.4052196145057678</v>
+        <v>0.5706554651260376</v>
       </c>
       <c r="D68">
-        <v>0.187014639377594</v>
+        <v>0.4053469002246856</v>
       </c>
       <c r="E68">
-        <v>0.1127944004929755</v>
+        <v>0.5075834393501282</v>
       </c>
       <c r="F68">
         <v>0.4052196145057678</v>
       </c>
       <c r="G68">
-        <v>0.1122087836265564</v>
+        <v>0.187014639377594</v>
       </c>
       <c r="H68">
-        <v>0.062036920338869</v>
+        <v>0.1127944004929755</v>
       </c>
       <c r="I68">
         <v>0.4052196145057678</v>
       </c>
       <c r="J68">
+        <v>0.1122087836265564</v>
+      </c>
+      <c r="K68">
+        <v>0.062036920338869</v>
+      </c>
+      <c r="L68">
+        <v>0.4052196145057678</v>
+      </c>
+      <c r="M68">
         <v>0.561043918132782</v>
       </c>
-      <c r="K68">
+      <c r="N68">
         <v>0.6203691959381104</v>
       </c>
-      <c r="L68" t="s">
-        <v>21</v>
-      </c>
-      <c r="M68" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="O68" t="s">
+        <v>24</v>
+      </c>
+      <c r="P68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69">
         <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C69">
-        <v>0.3387651145458221</v>
+        <v>0.5173241496086121</v>
       </c>
       <c r="D69">
-        <v>0.1673244196507665</v>
+        <v>0.3392743468284607</v>
       </c>
       <c r="E69">
-        <v>0.1023088934992955</v>
+        <v>0.4452615678310394</v>
       </c>
       <c r="F69">
         <v>0.3387651145458221</v>
       </c>
       <c r="G69">
-        <v>0.1003946512937545</v>
+        <v>0.1673244196507665</v>
       </c>
       <c r="H69">
-        <v>0.0562698915600776</v>
+        <v>0.1023088934992955</v>
       </c>
       <c r="I69">
         <v>0.3387651145458221</v>
       </c>
       <c r="J69">
+        <v>0.1003946512937545</v>
+      </c>
+      <c r="K69">
+        <v>0.0562698915600776</v>
+      </c>
+      <c r="L69">
+        <v>0.3387651145458221</v>
+      </c>
+      <c r="M69">
         <v>0.5019732713699341</v>
       </c>
-      <c r="K69">
+      <c r="N69">
         <v>0.5626989006996155</v>
       </c>
-      <c r="L69" t="s">
-        <v>21</v>
-      </c>
-      <c r="M69" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="O69" t="s">
+        <v>24</v>
+      </c>
+      <c r="P69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70">
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C70">
+        <v>0.2404200890382374</v>
+      </c>
+      <c r="D70">
+        <v>0.0752813916094138</v>
+      </c>
+      <c r="E70">
+        <v>0.1175833453943252</v>
+      </c>
+      <c r="F70">
         <v>0.07260147151975831</v>
       </c>
-      <c r="D70">
+      <c r="G70">
         <v>0.0468418813397615</v>
       </c>
-      <c r="E70">
+      <c r="H70">
         <v>0.0340422392498118</v>
       </c>
-      <c r="F70">
+      <c r="I70">
         <v>0.0752813916094138</v>
       </c>
-      <c r="G70">
+      <c r="J70">
         <v>0.0288554304926176</v>
       </c>
-      <c r="H70">
+      <c r="K70">
         <v>0.019061540710422</v>
       </c>
-      <c r="I70">
+      <c r="L70">
         <v>0.07135896311455441</v>
       </c>
-      <c r="J70">
+      <c r="M70">
         <v>0.1323198362812454</v>
       </c>
-      <c r="K70">
+      <c r="N70">
         <v>0.1728597183647615</v>
       </c>
-      <c r="L70" t="s">
-        <v>21</v>
-      </c>
-      <c r="M70" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="O70" t="s">
+        <v>24</v>
+      </c>
+      <c r="P70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71">
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C71">
+        <v>0.144010197845044</v>
+      </c>
+      <c r="D71">
+        <v>0.0016079520537933</v>
+      </c>
+      <c r="E71">
+        <v>0.0168576177336656</v>
+      </c>
+      <c r="F71">
         <v>0.0015592262339813</v>
       </c>
-      <c r="D71">
+      <c r="G71">
         <v>0.0070820658819489</v>
       </c>
-      <c r="E71">
+      <c r="H71">
         <v>0.0070489126913626</v>
       </c>
-      <c r="F71">
+      <c r="I71">
         <v>0.0016079520537933</v>
       </c>
-      <c r="G71">
+      <c r="J71">
         <v>0.0043560882911854</v>
       </c>
-      <c r="H71">
+      <c r="K71">
         <v>0.0039321736588218</v>
       </c>
-      <c r="I71">
+      <c r="L71">
         <v>0.0015348633240754</v>
       </c>
-      <c r="J71">
+      <c r="M71">
         <v>0.0200628563075573</v>
       </c>
-      <c r="K71">
+      <c r="N71">
         <v>0.036349461579691</v>
       </c>
-      <c r="L71" t="s">
-        <v>21</v>
-      </c>
-      <c r="M71" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="O71" t="s">
+        <v>24</v>
+      </c>
+      <c r="P71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72">
         <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C72">
+        <v>0.1439596978187424</v>
+      </c>
+      <c r="D72">
+        <v>0.0016079520537933</v>
+      </c>
+      <c r="E72">
+        <v>0.0168576177336656</v>
+      </c>
+      <c r="F72">
         <v>0.0015592262339813</v>
       </c>
-      <c r="D72">
+      <c r="G72">
         <v>0.0070820658819489</v>
       </c>
-      <c r="E72">
+      <c r="H72">
         <v>0.0070489126913626</v>
       </c>
-      <c r="F72">
+      <c r="I72">
         <v>0.0016079520537933</v>
       </c>
-      <c r="G72">
+      <c r="J72">
         <v>0.0043560882911854</v>
       </c>
-      <c r="H72">
+      <c r="K72">
         <v>0.0039321736588218</v>
       </c>
-      <c r="I72">
+      <c r="L72">
         <v>0.0015348633240754</v>
       </c>
-      <c r="J72">
+      <c r="M72">
         <v>0.0200628563075573</v>
       </c>
-      <c r="K72">
+      <c r="N72">
         <v>0.036349461579691</v>
       </c>
-      <c r="L72" t="s">
-        <v>21</v>
-      </c>
-      <c r="M72" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="O72" t="s">
+        <v>24</v>
+      </c>
+      <c r="P72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73">
         <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C73">
+        <v>0.1477136313915252</v>
+      </c>
+      <c r="D73">
         <v>0.001400381908752</v>
       </c>
-      <c r="D73">
-        <v>0.0068746018999566</v>
-      </c>
       <c r="E73">
-        <v>0.0087032001311621</v>
+        <v>0.0198261141777038</v>
       </c>
       <c r="F73">
         <v>0.001400381908752</v>
       </c>
       <c r="G73">
-        <v>0.0041247610934078</v>
+        <v>0.0068746018999566</v>
       </c>
       <c r="H73">
-        <v>0.0047867600806057</v>
+        <v>0.0087032001311621</v>
       </c>
       <c r="I73">
         <v>0.001400381908752</v>
       </c>
       <c r="J73">
+        <v>0.0041247610934078</v>
+      </c>
+      <c r="K73">
+        <v>0.0047867600806057</v>
+      </c>
+      <c r="L73">
+        <v>0.001400381908752</v>
+      </c>
+      <c r="M73">
         <v>0.0206238068640232</v>
       </c>
-      <c r="K73">
+      <c r="N73">
         <v>0.0478675998747348</v>
       </c>
-      <c r="L73" t="s">
-        <v>21</v>
-      </c>
-      <c r="M73" t="s">
-        <v>29</v>
+      <c r="O73" t="s">
+        <v>24</v>
+      </c>
+      <c r="P73" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>